<commit_message>
//updted excel runnmode= yes
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/TestData/Accural/LeaveBalance.xlsx
+++ b/leave/src/main/resources/TestData/Accural/LeaveBalance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\TestData\Accural\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Master\Automation_Project\leave\src\main\resources\TestData\Accural\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00A03C5-FDAE-40EA-92BE-9EE97AA97CCA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47BF5CA-CCA4-42B2-8181-CD82E7C309B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeaveBalance" sheetId="1" r:id="rId1"/>
@@ -1978,9 +1978,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:V124"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2066,7 +2066,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>145</v>
@@ -2134,7 +2134,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>146</v>
@@ -2202,7 +2202,7 @@
         <v>24</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>147</v>
@@ -2270,7 +2270,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>148</v>
@@ -2338,7 +2338,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>149</v>
@@ -2406,7 +2406,7 @@
         <v>27</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>150</v>
@@ -2474,7 +2474,7 @@
         <v>28</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>151</v>
@@ -2542,7 +2542,7 @@
         <v>29</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>152</v>
@@ -2610,7 +2610,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>276</v>
@@ -2678,7 +2678,7 @@
         <v>31</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>153</v>
@@ -2746,7 +2746,7 @@
         <v>32</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>154</v>
@@ -2814,7 +2814,7 @@
         <v>33</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>155</v>
@@ -2882,7 +2882,7 @@
         <v>34</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>156</v>
@@ -2950,7 +2950,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>157</v>
@@ -3018,7 +3018,7 @@
         <v>36</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>158</v>
@@ -3086,7 +3086,7 @@
         <v>37</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>159</v>
@@ -3154,7 +3154,7 @@
         <v>38</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>160</v>
@@ -3222,7 +3222,7 @@
         <v>39</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>161</v>
@@ -3290,7 +3290,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>162</v>
@@ -3358,7 +3358,7 @@
         <v>41</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>163</v>
@@ -3426,7 +3426,7 @@
         <v>42</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>164</v>
@@ -3494,7 +3494,7 @@
         <v>43</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>165</v>
@@ -3562,7 +3562,7 @@
         <v>44</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>166</v>
@@ -3630,7 +3630,7 @@
         <v>45</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>167</v>
@@ -3698,7 +3698,7 @@
         <v>46</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>168</v>
@@ -3766,7 +3766,7 @@
         <v>47</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>169</v>
@@ -3834,7 +3834,7 @@
         <v>48</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>170</v>
@@ -3902,7 +3902,7 @@
         <v>49</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>171</v>
@@ -3970,7 +3970,7 @@
         <v>50</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>172</v>
@@ -4038,7 +4038,7 @@
         <v>51</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>173</v>
@@ -4106,7 +4106,7 @@
         <v>52</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>174</v>
@@ -4174,7 +4174,7 @@
         <v>53</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>175</v>
@@ -4242,7 +4242,7 @@
         <v>54</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>176</v>
@@ -4310,7 +4310,7 @@
         <v>55</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>177</v>
@@ -4378,7 +4378,7 @@
         <v>56</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>178</v>
@@ -4446,7 +4446,7 @@
         <v>57</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>179</v>
@@ -4514,7 +4514,7 @@
         <v>58</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>180</v>
@@ -4582,7 +4582,7 @@
         <v>59</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>181</v>
@@ -4650,7 +4650,7 @@
         <v>60</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>182</v>
@@ -4718,7 +4718,7 @@
         <v>61</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>183</v>
@@ -4786,7 +4786,7 @@
         <v>62</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>184</v>
@@ -7642,7 +7642,7 @@
         <v>104</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>226</v>
@@ -7710,7 +7710,7 @@
         <v>105</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>227</v>
@@ -7778,7 +7778,7 @@
         <v>106</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>228</v>
@@ -7846,7 +7846,7 @@
         <v>107</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>229</v>
@@ -7914,7 +7914,7 @@
         <v>108</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>230</v>
@@ -7982,7 +7982,7 @@
         <v>109</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>231</v>
@@ -8050,7 +8050,7 @@
         <v>110</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>232</v>
@@ -8118,7 +8118,7 @@
         <v>111</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>233</v>
@@ -8186,7 +8186,7 @@
         <v>112</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>234</v>
@@ -8254,7 +8254,7 @@
         <v>113</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D93" s="3" t="s">
         <v>235</v>
@@ -8322,7 +8322,7 @@
         <v>114</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D94" s="3" t="s">
         <v>236</v>
@@ -8390,7 +8390,7 @@
         <v>115</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D95" s="3" t="s">
         <v>237</v>
@@ -8458,7 +8458,7 @@
         <v>116</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D96" s="3" t="s">
         <v>238</v>
@@ -8526,7 +8526,7 @@
         <v>117</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D97" s="3" t="s">
         <v>239</v>
@@ -8594,7 +8594,7 @@
         <v>118</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>240</v>
@@ -8662,7 +8662,7 @@
         <v>119</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D99" s="3" t="s">
         <v>241</v>
@@ -8730,7 +8730,7 @@
         <v>120</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>242</v>
@@ -8798,7 +8798,7 @@
         <v>121</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>243</v>
@@ -10440,8 +10440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F6D715-F1A2-4992-BE3D-118FEE3675AA}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>